<commit_message>
added super basic instructions
</commit_message>
<xml_diff>
--- a/BOM/BOM_TinyGawant_RevC.xlsx
+++ b/BOM/BOM_TinyGawant_RevC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arko/Desktop/TinyGawant_temp/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arko/Documents/N6ARA Electronics/GitHub/TinyGawant/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D265400-5A46-1F49-ABEB-3736C9278753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C763D86C-4728-C342-BA88-EBFC163B200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="4580" windowWidth="28040" windowHeight="17440" xr2:uid="{AE5E156E-F7C5-F840-9AF4-BD052DCDC38D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Reference</t>
   </si>
@@ -125,9 +125,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>CBM-443BF</t>
   </si>
   <si>
@@ -137,21 +134,12 @@
     <t>https://www.aliexpress.us/item/2255800609195661.html?spm=a2g0o.productlist.main.1.4ba9unA0unA0IK&amp;algo_pvid=9f4554e2-11d2-4adb-a82a-5c57be2beff6&amp;algo_exp_id=9f4554e2-11d2-4adb-a82a-5c57be2beff6-0&amp;pdp_ext_f=%7B%22order%22%3A%2219%22%2C%22eval%22%3A%221%22%2C%22fromPage%22%3A%22search%22%7D&amp;pdp_npi=6%40dis%21USD%219.55%219.55%21%21%219.55%219.55%21%40210325a917660290419132931edb34%2112000030048704721%21sea%21US%213483570996%21X%211%210%21n_tag%3A-29919%3Bd%3A486aba74%3Bm03_new_user%3A-29895&amp;curPageLogUid=80i4KDQZDI0j&amp;utparam-url=scene%3Asearch%7Cquery_from%3A%7Cx_object_id%3A4000795510413%7C_p_origin_prod%3A</t>
   </si>
   <si>
-    <t>Digikey Cart</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
     <t>JLCPCB</t>
   </si>
   <si>
-    <t>Red Wire</t>
-  </si>
-  <si>
-    <t>Green Wire</t>
-  </si>
-  <si>
     <t>Antenna</t>
   </si>
   <si>
@@ -201,6 +189,63 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>26AWG Green Enamel Wire</t>
+  </si>
+  <si>
+    <t>24AWG Red Enamel Wire</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/BNTECHGO-AWG-Magnet-Wire-Transformers/dp/B07DYHWLN4/ref=sr_1_5?dib=eyJ2IjoiMSJ9.T3Ul6AAFydmV-d_-CiWqSOo4gGqiz7pPGX4uu-tgp91Uz8UDmDqH8WcqGDNCB0nASmRUuhfX4iN0RZakJU07DzAEplyXYHcojTMP4m3FGJ5JPHVgh9WsCtBBpnL-l5gtozaZ1Zccg2B47I56QOWE9TdXpyhM0Vq-aou5cLVF9d2If9T7cT1eBVhsQfHPZ0qK1IjkOvqHsRwgkZCcfU0RhXIqun1H3sMrp-vOuHH7bHs.keJAopHhCjqzf_ORW6_Log1OwxKHoD8gj3qxIPjLaFU&amp;dib_tag=se&amp;keywords=enameled%2Bcopper%2Bwire&amp;qid=1766271692&amp;sr=8-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/BNTECHGO-AWG-Magnet-Wire-Transformers/dp/B07HRKKMPS/ref=sr_1_7_sspa?crid=12PVFVFD45WC4&amp;dib=eyJ2IjoiMSJ9.GfGCp1Wvx140pjLuMz3aI6wPrbZKYdBhCtRZ81xGu0XV6En0x5usAIXu_J4MJaXPsP8uD7tngx8WYsTls0IkxnFTFDnihgmKaGvu-rIKCmCyTX7a91kWyUFfrHj6u5lWP90B42q8rxUwtCxCaqo-L1I87Z-IyXnA_l0naAeAXoElYpJOL3EA33wngyAXwEBi08_0SWSdL1r4gnfuAwbsb6yLQ70njgJULhZOC5WoDEk.dYYUVAtyiKCv2QUEBzB8P9SjXI8Gwk2B3BbFux3aPSo&amp;dib_tag=se&amp;keywords=enameled%2Bwire%2Bgreen&amp;qid=1766271862&amp;sprefix=enameled%2Bwire%2Bgreen%2Caps%2C223&amp;sr=8-7-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9tdGY&amp;th=1</t>
+  </si>
+  <si>
+    <t>Get quote at JLCPCB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC21X7R103J50NT/22577164</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/comchip-technology/CDBW46-G/3308556</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/würth-elektronik/156125RS57000/9857918</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/TZMC3V3-GS08/3104272</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/7790/2171010</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CRM2512-FX-51R0ELF/4698407</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0805FR-071KL/727444</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/JS202011AQN/1640096</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/JS102011SAQN/1640095</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (per board at volume, total cost may vary minimum quantity buy and shipping)</t>
+  </si>
+  <si>
+    <t>Cost per Unit</t>
+  </si>
+  <si>
+    <t>3D Print Files</t>
+  </si>
+  <si>
+    <t>See "3D Printables" Folder</t>
   </si>
 </sst>
 </file>
@@ -1105,16 +1150,16 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="101.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1131,10 +1176,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1155,7 +1200,7 @@
         <v>0.2</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1176,7 +1221,7 @@
         <v>0.26</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1197,7 +1242,7 @@
         <v>0.42</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1218,7 +1263,7 @@
         <v>0.13</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1239,7 +1284,7 @@
         <v>1.28</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1260,7 +1305,7 @@
         <v>1.56</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1281,7 +1326,7 @@
         <v>0.12</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1302,7 +1347,7 @@
         <v>0.75</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1323,7 +1368,7 @@
         <v>0.76</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1335,13 +1380,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="4">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1353,14 +1398,14 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" s="4">
         <f>157/100</f>
         <v>1.57</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1372,139 +1417,174 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.1</v>
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.1</v>
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4">
         <v>1.8759999999999999</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E18" s="4">
         <v>0.9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E19" s="4">
         <v>0.1</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E20" s="4">
         <f>0.1*C20</f>
         <v>0.2</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E21" s="4">
         <f>0.1*C21</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E24" s="4">
         <f>SUM(E2:E21)</f>
-        <v>14.625999999999999</v>
+        <v>14.426</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update to Rev C Production
</commit_message>
<xml_diff>
--- a/BOM/BOM_TinyGawant_RevC.xlsx
+++ b/BOM/BOM_TinyGawant_RevC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arko/Documents/N6ARA Electronics/GitHub/TinyGawant/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C763D86C-4728-C342-BA88-EBFC163B200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C8BF04-1B7D-A248-98F2-D22A5858F62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="4580" windowWidth="28040" windowHeight="17440" xr2:uid="{AE5E156E-F7C5-F840-9AF4-BD052DCDC38D}"/>
+    <workbookView xWindow="2340" yWindow="4280" windowWidth="28040" windowHeight="17440" xr2:uid="{AE5E156E-F7C5-F840-9AF4-BD052DCDC38D}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_TinyGawant_RevC" sheetId="1" r:id="rId1"/>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,7 +1510,7 @@
         <v>45</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>45</v>

</xml_diff>